<commit_message>
next parts of grid
</commit_message>
<xml_diff>
--- a/Assignment2/AndrewDodgeA2-grid.xlsx
+++ b/Assignment2/AndrewDodgeA2-grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RoyalD\Documents\Class\4004 - Software Quality Assurance\Assignments\Comp4004\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC362AE-63E5-4D6E-9FE8-E91D5CBB3EEB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016ECF65-24A9-460F-809E-A166578944A8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="166">
   <si>
     <t>First Name</t>
   </si>
@@ -2085,8 +2085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2746,13 +2746,15 @@
         <v>35</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="12">
         <v>0.5</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F28" s="29"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -2769,13 +2771,15 @@
         <v>36</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="12">
         <v>0.5</v>
       </c>
-      <c r="E29" s="29"/>
+      <c r="E29" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F29" s="29"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -2792,13 +2796,15 @@
         <v>37</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="12">
         <v>0.5</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F30" s="29"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
@@ -2815,13 +2821,15 @@
         <v>38</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="12">
         <v>0.5</v>
       </c>
-      <c r="E31" s="29"/>
+      <c r="E31" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F31" s="29"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
@@ -2837,13 +2845,15 @@
         <v>39</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="12">
         <v>0.5</v>
       </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F32" s="29"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
@@ -2860,13 +2870,15 @@
         <v>40</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="12">
         <v>0.5</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F33" s="29"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -2883,13 +2895,15 @@
         <v>41</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="12">
         <v>0.5</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F34" s="29"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
@@ -2906,13 +2920,15 @@
         <v>42</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="12">
         <v>0.5</v>
       </c>
-      <c r="E35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F35" s="29"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
@@ -2929,13 +2945,15 @@
         <v>44</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="12">
         <v>0.5</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="E36" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F36" s="29"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
@@ -2952,13 +2970,15 @@
         <v>45</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="12">
         <v>0.5</v>
       </c>
-      <c r="E37" s="29"/>
+      <c r="E37" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F37" s="29"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -2975,13 +2995,15 @@
         <v>46</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="12">
         <v>0.5</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F38" s="29"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
@@ -2998,13 +3020,15 @@
         <v>47</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="12">
         <v>0.5</v>
       </c>
-      <c r="E39" s="29"/>
+      <c r="E39" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F39" s="29"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
@@ -3021,13 +3045,15 @@
         <v>48</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C40" s="23"/>
       <c r="D40" s="12">
         <v>0.5</v>
       </c>
-      <c r="E40" s="29"/>
+      <c r="E40" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F40" s="29"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -3044,13 +3070,15 @@
         <v>49</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C41" s="23"/>
       <c r="D41" s="12">
         <v>0.5</v>
       </c>
-      <c r="E41" s="29"/>
+      <c r="E41" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F41" s="29"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -3067,13 +3095,15 @@
         <v>50</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>5</v>
+        <v>154</v>
       </c>
       <c r="C42" s="23"/>
       <c r="D42" s="12">
         <v>0.5</v>
       </c>
-      <c r="E42" s="29"/>
+      <c r="E42" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="F42" s="29"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>

</xml_diff>

<commit_message>
Up to line 122
</commit_message>
<xml_diff>
--- a/Assignment2/AndrewDodgeA2-grid.xlsx
+++ b/Assignment2/AndrewDodgeA2-grid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RoyalD\Documents\Class\4004 - Software Quality Assurance\Assignments\Comp4004\Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0576A9F4-16FD-4395-A44B-D662C2D26664}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E592A29-3867-48AF-ACEA-625A2EB803DF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2108,7 +2108,7 @@
   <dimension ref="A1:IV152"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A104" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4952,8 +4952,8 @@
       <c r="A119" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B119" s="22" t="s">
-        <v>5</v>
+      <c r="B119" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="C119" s="23"/>
       <c r="D119" s="12">

</xml_diff>